<commit_message>
more slides filled out, minor edits to paper, energy detector results added to excel spreadsheet
</commit_message>
<xml_diff>
--- a/results/FAM_timings.xlsx
+++ b/results/FAM_timings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="22815" windowHeight="8640"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="19440" windowHeight="8640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FAM" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t>Matlab Timings</t>
   </si>
@@ -73,6 +73,63 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>25% Overlap</t>
+  </si>
+  <si>
+    <t>50% Overlap</t>
+  </si>
+  <si>
+    <t>75% Overlap</t>
+  </si>
+  <si>
+    <t>CUDA Speedup Over Matlab</t>
+  </si>
+  <si>
+    <t>10.72x</t>
+  </si>
+  <si>
+    <t>15.57x</t>
+  </si>
+  <si>
+    <t>29.31x</t>
+  </si>
+  <si>
+    <t>6.82x</t>
+  </si>
+  <si>
+    <t>9.71x</t>
+  </si>
+  <si>
+    <t>17.29x</t>
+  </si>
+  <si>
+    <t>7.46x</t>
+  </si>
+  <si>
+    <t>16.77x</t>
+  </si>
+  <si>
+    <t>16.99x</t>
+  </si>
+  <si>
+    <t>5.12x</t>
+  </si>
+  <si>
+    <t>6.38x</t>
+  </si>
+  <si>
+    <t>10.12x</t>
+  </si>
+  <si>
+    <t>Matlab Timngs (msec)</t>
+  </si>
+  <si>
+    <t>CUDA Timngs (msec)</t>
   </si>
 </sst>
 </file>
@@ -88,15 +145,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -104,19 +167,139 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E7" headerRowCount="0" headerRowDxfId="17">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Matlab Timings" totalsRowLabel="Total" headerRowDxfId="12"/>
+    <tableColumn id="2" name="Column1" headerRowDxfId="13"/>
+    <tableColumn id="3" name="Column2" headerRowDxfId="14"/>
+    <tableColumn id="4" name="Column3" headerRowDxfId="15"/>
+    <tableColumn id="5" name="Column4" totalsRowFunction="sum" headerRowDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A11:E14" headerRowCount="0" headerRowDxfId="6">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Matlab Timings" totalsRowLabel="Total" headerRowDxfId="11"/>
+    <tableColumn id="2" name="Column1" headerRowDxfId="10"/>
+    <tableColumn id="3" name="Column2" headerRowDxfId="9"/>
+    <tableColumn id="4" name="Column3" headerRowDxfId="8"/>
+    <tableColumn id="5" name="Column4" totalsRowFunction="sum" headerRowDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A18:E21" headerRowCount="0" headerRowDxfId="0">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Matlab Timings" totalsRowLabel="Total" headerRowDxfId="5"/>
+    <tableColumn id="2" name="Column1" headerRowDxfId="4"/>
+    <tableColumn id="3" name="Column2" headerRowDxfId="3"/>
+    <tableColumn id="4" name="Column3" headerRowDxfId="2"/>
+    <tableColumn id="5" name="Column4" totalsRowFunction="sum" headerRowDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
@@ -1706,28 +1889,274 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1">
+        <v>512</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2048</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>15.987</v>
+      </c>
+      <c r="C5">
+        <v>10.196</v>
+      </c>
+      <c r="D5">
+        <v>11.523</v>
+      </c>
+      <c r="E5">
+        <v>8.6560000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>22.818000000000001</v>
+      </c>
+      <c r="C6">
+        <v>14.17</v>
+      </c>
+      <c r="D6">
+        <v>26.37</v>
+      </c>
+      <c r="E6">
+        <v>10.817</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>42.716999999999999</v>
+      </c>
+      <c r="C7">
+        <v>25.283999999999999</v>
+      </c>
+      <c r="D7">
+        <v>26.428000000000001</v>
+      </c>
+      <c r="E7">
+        <v>17.408999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>512</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2048</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>1.49</v>
+      </c>
+      <c r="C12">
+        <v>1.494</v>
+      </c>
+      <c r="D12">
+        <v>1.5429999999999999</v>
+      </c>
+      <c r="E12">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="C13">
+        <v>1.4590000000000001</v>
+      </c>
+      <c r="D13">
+        <v>1.5720000000000001</v>
+      </c>
+      <c r="E13">
+        <v>1.6930000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>1.4570000000000001</v>
+      </c>
+      <c r="C14">
+        <v>1.462</v>
+      </c>
+      <c r="D14">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="E14">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1">
+        <v>512</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2048</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="G22" s="4"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A17:E17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>